<commit_message>
fix multi answers in single evaluation
</commit_message>
<xml_diff>
--- a/csv/fellows_progress.xlsx
+++ b/csv/fellows_progress.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
   <si>
     <t>Nombre</t>
   </si>
@@ -29,33 +29,33 @@
     <t>Módulo actual</t>
   </si>
   <si>
-    <t>Andre</t>
-  </si>
-  <si>
-    <t>andre@fcb.com</t>
-  </si>
-  <si>
-    <t>Desarrollo Sostenible: Agenda 2030 (segunda parte)</t>
-  </si>
-  <si>
     <t>Alejandro May Guillén</t>
   </si>
   <si>
     <t>alejandromyg@gmail.com</t>
   </si>
   <si>
+    <t>Conceptos básicos en torno a la incidencia en políticas públicas</t>
+  </si>
+  <si>
     <t>Alicia Mateos Guzmán</t>
   </si>
   <si>
     <t>aliciamateosguzman@gmail.com</t>
   </si>
   <si>
+    <t>GOBIERNO ABIERTO Y LA AGENDA 2030 PARA EL DESARROLLO SOSTENIBLE</t>
+  </si>
+  <si>
     <t>Antonio Atempa Tuxpan</t>
   </si>
   <si>
     <t>uxpa01@hotmail.com</t>
   </si>
   <si>
+    <t>Gobierno abierto como herramienta y plataforma para la incidencia (segunda parte); Metodología de Marco Lógico (evaluación final)</t>
+  </si>
+  <si>
     <t>Antonio Carrillo Bolea</t>
   </si>
   <si>
@@ -68,15 +68,15 @@
     <t>atenas.hdez@gmail.com</t>
   </si>
   <si>
-    <t>Desarrollo Sostenible: Agenda 2030 (primera parte); Metodología de Marco Lógico (segunda parte</t>
-  </si>
-  <si>
     <t>César Francisco Zamora Salazar</t>
   </si>
   <si>
     <t>czasalazar@gmail.com</t>
   </si>
   <si>
+    <t>Gobierno abierto como herramienta y plataforma para la incidencia (primera parte); Metodología de Marco Lógico (séptima parte)</t>
+  </si>
+  <si>
     <t>Claudia Sarahí Soriano Melo</t>
   </si>
   <si>
@@ -95,10 +95,7 @@
     <t>DROSEMBERGC@GMAIL.COM</t>
   </si>
   <si>
-    <t>Primer Seminario "Gobierno Abierto desde lo Local para el Desarrollo Sostenible", Mazatlán, Sinaloa, del 6 al 8 de junio</t>
-  </si>
-  <si>
-    <t>Evelyn</t>
+    <t>Evelyn Cruz Mendoza</t>
   </si>
   <si>
     <t>burundanga_bnd@hotmail.com</t>
@@ -116,6 +113,9 @@
     <t>gerardo.martinez.villanueva@gmail.com</t>
   </si>
   <si>
+    <t>Gobierno Abierto en la práctica mexicana (segunda parte)</t>
+  </si>
+  <si>
     <t>Gerardo Javier Vilet Espinosa</t>
   </si>
   <si>
@@ -140,6 +140,9 @@
     <t>jaciel.hernandez@durango.gob.mx</t>
   </si>
   <si>
+    <t>Desarrollo Sostenible: Localizando los ODS (primera parte); Matriz de Marco Lógico (cuarta parte)</t>
+  </si>
+  <si>
     <t>JIMENA GARCIA CHAVEZ</t>
   </si>
   <si>
@@ -152,6 +155,9 @@
     <t>fabila.jorge@hotmail.com</t>
   </si>
   <si>
+    <t>Gobierno Abierto como concepto (primera parte); metodología de Marco Lógico (quinta parte)</t>
+  </si>
+  <si>
     <t>JORGE GABRIEL GASCA SANTOS</t>
   </si>
   <si>
@@ -206,7 +212,7 @@
     <t>mleon@iniciativasinaloa.org.mx</t>
   </si>
   <si>
-    <t>Alejandro Pérezrabelo García</t>
+    <t>Alejandro Rabelo García</t>
   </si>
   <si>
     <t>acrofobos@gmail.com</t>
@@ -246,6 +252,9 @@
   </si>
   <si>
     <t>thelma.beltran@gmail.com</t>
+  </si>
+  <si>
+    <t>Desarrollo Sostenible: ODS 16 (primera parte); Metodología de Marco Lógico (tercera parte)</t>
   </si>
   <si>
     <t>VERÓNICA GALLEGOS GÓMEZ</t>
@@ -639,7 +648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -650,7 +659,7 @@
     <col min="1" max="1" width="42.418213" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="44.703369" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="142.679443" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="153.248291" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -675,7 +684,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -689,35 +698,35 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -725,69 +734,69 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -795,55 +804,55 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -851,13 +860,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -865,13 +874,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -879,97 +888,97 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -977,27 +986,27 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -1005,13 +1014,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1019,41 +1028,41 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1061,41 +1070,41 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
@@ -1103,69 +1112,69 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1173,72 +1182,58 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42">
-        <v>3</v>
-      </c>
-      <c r="D42" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>